<commit_message>
More SAM models integrated
</commit_message>
<xml_diff>
--- a/SAM_flatJSON/SAM_comb.xlsx
+++ b/SAM_flatJSON/SAM_comb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzrfl\Documents\GitHub\DOE_CSP_PROJECT\SAM_flatJSON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOE_CSP_PROJECT\SAM_flatJSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC2EDDB-D5C4-480B-99B3-FB092BC8B5AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC4CBF6-E190-47F8-9348-9860AA3E4C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="1080" windowWidth="21600" windowHeight="12915" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
+    <workbookView xWindow="7995" yWindow="1815" windowWidth="21600" windowHeight="12915" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="97">
   <si>
     <t>CSP</t>
   </si>
@@ -226,6 +226,102 @@
   </si>
   <si>
     <t>Possible combinations for SAM</t>
+  </si>
+  <si>
+    <t>tcstrough_physical_utilityrate5</t>
+  </si>
+  <si>
+    <t>cashloan_inputs</t>
+  </si>
+  <si>
+    <t>elec_cost_without_system_year1</t>
+  </si>
+  <si>
+    <t>elec_cost_with_system_year1</t>
+  </si>
+  <si>
+    <t>savings_year1</t>
+  </si>
+  <si>
+    <t>npv</t>
+  </si>
+  <si>
+    <t>payback</t>
+  </si>
+  <si>
+    <t>discounted_payback</t>
+  </si>
+  <si>
+    <t>adjusted_installed_cost</t>
+  </si>
+  <si>
+    <t>first_cost</t>
+  </si>
+  <si>
+    <t>loan_amount</t>
+  </si>
+  <si>
+    <t>tcstrough_physical_levpartflip</t>
+  </si>
+  <si>
+    <t>tax_investor_aftertax_irr</t>
+  </si>
+  <si>
+    <t>tax_investor_aftertax_npv</t>
+  </si>
+  <si>
+    <t>sponsor_aftertax_irr</t>
+  </si>
+  <si>
+    <t>sponsor_aftertax_npv</t>
+  </si>
+  <si>
+    <t>tcstrough_physical_equpartflip</t>
+  </si>
+  <si>
+    <t>tcstrough_physical_saleleaseback</t>
+  </si>
+  <si>
+    <t>adjusted_cost_installed</t>
+  </si>
+  <si>
+    <t>tcslinear_fresnel_lcoefcr</t>
+  </si>
+  <si>
+    <t>tcslinear_fresnel_saleleaseback</t>
+  </si>
+  <si>
+    <t>tcslinear_fresnel_none</t>
+  </si>
+  <si>
+    <t>tcslinear_fresnel_levpartflip</t>
+  </si>
+  <si>
+    <t>tcslinear_fresnel_utilityrate5</t>
+  </si>
+  <si>
+    <t>tcslinear_fresnel_equpartflip</t>
+  </si>
+  <si>
+    <t>tcsmolten_salt_levpartflip</t>
+  </si>
+  <si>
+    <t>tcsmolten_salt_saleleaseback</t>
+  </si>
+  <si>
+    <t>tcsmolten_salt_equpartflip</t>
+  </si>
+  <si>
+    <t>tcsdirect_steam_singleowner</t>
+  </si>
+  <si>
+    <t>tcsdirect_steam_levpartflip</t>
+  </si>
+  <si>
+    <t>tcsdirect_steam_equpartflip</t>
+  </si>
+  <si>
+    <t>tcsdirect_steam_saleleaseback</t>
   </si>
 </sst>
 </file>
@@ -651,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2441DE-F27B-4F1C-970B-4AC464B11485}">
   <dimension ref="A1:Y57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +847,9 @@
         <f t="shared" ref="F4:F5" si="0">CONCATENATE(E4,"_inputs")</f>
         <v>utilityrate5_inputs</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -939,55 +1038,187 @@
       <c r="Y13" s="15"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q14" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="T14" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="U14" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="V14" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W14" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
+      <c r="D15" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q15" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="R15" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="S15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="T15" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
+      <c r="D16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="S16" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="T16" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="U16" s="15" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="17" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
@@ -1031,21 +1262,63 @@
       <c r="Y17" s="15"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
+      <c r="D18" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="P18" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q18" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="R18" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="S18" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="T18" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="U18" s="15" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="19" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
@@ -1161,11 +1434,14 @@
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="13" t="s">
         <v>11</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
@@ -1178,11 +1454,14 @@
       <c r="N22" s="15"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="13" t="s">
         <v>23</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
@@ -1195,11 +1474,14 @@
       <c r="N23" s="15"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="13" t="s">
         <v>24</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -1212,11 +1494,14 @@
       <c r="N24" s="15"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="13" t="s">
         <v>25</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -1229,11 +1514,14 @@
       <c r="N25" s="15"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="13" t="s">
         <v>26</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -1246,11 +1534,14 @@
       <c r="N26" s="15"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="13" t="s">
         <v>40</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -1463,11 +1754,14 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="13" t="s">
         <v>11</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
@@ -1480,11 +1774,14 @@
       <c r="N38" s="15"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="13" t="s">
         <v>24</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
@@ -1497,11 +1794,14 @@
       <c r="N39" s="15"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="13" t="s">
         <v>26</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
@@ -1525,11 +1825,14 @@
       <c r="N41" s="15"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="13" t="s">
         <v>10</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>93</v>
       </c>
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
@@ -1548,6 +1851,9 @@
       <c r="B43" s="10" t="s">
         <v>11</v>
       </c>
+      <c r="D43" s="16" t="s">
+        <v>94</v>
+      </c>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
@@ -1565,6 +1871,9 @@
       <c r="B44" s="10" t="s">
         <v>24</v>
       </c>
+      <c r="D44" s="16" t="s">
+        <v>95</v>
+      </c>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
@@ -1581,6 +1890,9 @@
       </c>
       <c r="B45" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
@@ -1756,5 +2068,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More SAM model integrated
</commit_message>
<xml_diff>
--- a/SAM_flatJSON/SAM_comb.xlsx
+++ b/SAM_flatJSON/SAM_comb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOE_CSP_PROJECT\SAM_flatJSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC4CBF6-E190-47F8-9348-9860AA3E4C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424C1DE9-BD56-4044-A005-A9909A2E16F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7995" yWindow="1815" windowWidth="21600" windowHeight="12915" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
+    <workbookView xWindow="5280" yWindow="1410" windowWidth="21600" windowHeight="12915" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="110">
   <si>
     <t>CSP</t>
   </si>
@@ -322,6 +322,45 @@
   </si>
   <si>
     <t>tcsdirect_steam_saleleaseback</t>
+  </si>
+  <si>
+    <t>trough_physical_process_heat_none</t>
+  </si>
+  <si>
+    <t>iph_to_lcoefcr</t>
+  </si>
+  <si>
+    <t>trough_physical_process_heat_iph_to_lcoefcr</t>
+  </si>
+  <si>
+    <t>tcsiscc_singleowner</t>
+  </si>
+  <si>
+    <t>tcsMSLF_singleowner</t>
+  </si>
+  <si>
+    <t>tcsMSLF_levpartflip</t>
+  </si>
+  <si>
+    <t>tcsMSLF_equpartflip</t>
+  </si>
+  <si>
+    <t>tcsMSLF_utilityrate5</t>
+  </si>
+  <si>
+    <t>tcsMSLF_lcoefcr</t>
+  </si>
+  <si>
+    <t>tcsMSLF_saleleaseback</t>
+  </si>
+  <si>
+    <t>tcsMSLF_none</t>
+  </si>
+  <si>
+    <t>linear_fresnel_dsg_iph_iph_to_lcoefcr</t>
+  </si>
+  <si>
+    <t>linear_fresnel_dsg_iph_none</t>
   </si>
 </sst>
 </file>
@@ -745,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2441DE-F27B-4F1C-970B-4AC464B11485}">
-  <dimension ref="A1:Y57"/>
+  <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:B42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,6 +970,12 @@
       <c r="D8" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="E8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1571,6 +1616,9 @@
       <c r="B29" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="D29" s="14" t="s">
+        <v>101</v>
+      </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
@@ -1588,6 +1636,9 @@
       <c r="B30" s="10" t="s">
         <v>11</v>
       </c>
+      <c r="D30" s="14" t="s">
+        <v>102</v>
+      </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
@@ -1605,6 +1656,9 @@
       <c r="B31" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="D31" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -1622,6 +1676,9 @@
       <c r="B32" s="10" t="s">
         <v>24</v>
       </c>
+      <c r="D32" s="14" t="s">
+        <v>103</v>
+      </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -1639,6 +1696,9 @@
       <c r="B33" s="10" t="s">
         <v>25</v>
       </c>
+      <c r="D33" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
@@ -1656,6 +1716,9 @@
       <c r="B34" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="D34" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
@@ -1672,6 +1735,9 @@
       </c>
       <c r="B35" s="10" t="s">
         <v>40</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
@@ -1814,6 +1880,7 @@
       <c r="N40" s="15"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D41" s="14"/>
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
@@ -1845,10 +1912,10 @@
       <c r="N42" s="15"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="16" t="s">
@@ -1865,10 +1932,10 @@
       <c r="N43" s="15"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="16" t="s">
@@ -1885,10 +1952,10 @@
       <c r="N44" s="15"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D45" s="16" t="s">
@@ -1905,6 +1972,7 @@
       <c r="N45" s="15"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D46" s="14"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
@@ -1916,11 +1984,14 @@
       <c r="N46" s="15"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="13" t="s">
         <v>10</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
@@ -1933,6 +2004,7 @@
       <c r="N47" s="15"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D48" s="14"/>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
@@ -1944,11 +2016,14 @@
       <c r="N48" s="15"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="13" t="s">
         <v>41</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
@@ -1961,11 +2036,14 @@
       <c r="N49" s="15"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="13" t="s">
         <v>40</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="F50" s="15"/>
       <c r="G50" s="15"/>
@@ -1978,6 +2056,7 @@
       <c r="N50" s="15"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D51" s="14"/>
       <c r="F51" s="15"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
@@ -1989,11 +2068,14 @@
       <c r="N51" s="15"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="13" t="s">
         <v>41</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="F52" s="15"/>
       <c r="G52" s="15"/>
@@ -2006,11 +2088,14 @@
       <c r="N52" s="15"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="13" t="s">
         <v>40</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>109</v>
       </c>
       <c r="F53" s="15"/>
       <c r="G53" s="15"/>
@@ -2023,6 +2108,7 @@
       <c r="N53" s="15"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D54" s="14"/>
       <c r="F54" s="15"/>
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
@@ -2034,6 +2120,7 @@
       <c r="N54" s="15"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D55" s="14"/>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
@@ -2045,6 +2132,7 @@
       <c r="N55" s="15"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D56" s="14"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
@@ -2056,6 +2144,7 @@
       <c r="N56" s="15"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D57" s="14"/>
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
@@ -2066,6 +2155,12 @@
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
     </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D58" s="14"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D59" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Desal cost model added
Cost model for VAGMD, good to use.
</commit_message>
<xml_diff>
--- a/SAM_flatJSON/SAM_comb.xlsx
+++ b/SAM_flatJSON/SAM_comb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzrfl\Documents\GitHub\DOE_CSP_PROJECT\SAM_flatJSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6AC216-C4E4-40ED-B5F7-91731CF2E3A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBB0E77-39D8-4AB2-9678-797B432ACCB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="825" windowWidth="12810" windowHeight="12210" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="18615" windowHeight="13200" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="113">
   <si>
     <t>CSP</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>VAGMD</t>
+  </si>
+  <si>
+    <t>Desal in Python</t>
   </si>
 </sst>
 </file>
@@ -793,7 +796,7 @@
   <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +836,7 @@
         <v>110</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update based on the meeting with Adam on March 13th,2020
Including initial implement of RO model.
</commit_message>
<xml_diff>
--- a/SAM_flatJSON/SAM_comb.xlsx
+++ b/SAM_flatJSON/SAM_comb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzrfl\Documents\GitHub\DOE_CSP_PROJECT\SAM_flatJSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBB0E77-39D8-4AB2-9678-797B432ACCB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E733EAE-03FA-423F-BA42-BDB9C8A33B64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="18615" windowHeight="13200" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
+    <workbookView xWindow="10215" yWindow="2190" windowWidth="16545" windowHeight="11385" xr2:uid="{0AB9CDDA-9527-4E50-AF91-EAE24BFA8DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="115">
   <si>
     <t>CSP</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>Desal in Python</t>
+  </si>
+  <si>
+    <t>PV detailed</t>
+  </si>
+  <si>
+    <t>pvsamv1</t>
   </si>
 </sst>
 </file>
@@ -793,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2441DE-F27B-4F1C-970B-4AC464B11485}">
-  <dimension ref="A1:Y59"/>
+  <dimension ref="A1:Y60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +926,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="3" t="str">
-        <f t="shared" ref="C5:C9" si="1">CONCATENATE(B5,"_inputs")</f>
+        <f t="shared" ref="C5:C10" si="1">CONCATENATE(B5,"_inputs")</f>
         <v>tcsmolten_salt_inputs</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1011,109 +1017,57 @@
         <v>linear_fresnel_dsg_iph_inputs</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>pvsamv1_inputs</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-    </row>
-    <row r="13" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="O13" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="P13" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q13" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R13" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="S13" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="T13" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="U13" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E13" s="7"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="14"/>
+        <v>10</v>
+      </c>
       <c r="D14" s="14" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="F14" s="15" t="s">
         <v>44</v>
@@ -1143,42 +1097,41 @@
         <v>54</v>
       </c>
       <c r="O14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="P14" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="Q14" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="Q14" s="15" t="s">
-        <v>77</v>
-      </c>
       <c r="R14" s="15" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="S14" s="15" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="T14" s="15" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="U14" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="V14" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="W14" s="15" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>23</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C15" s="14"/>
       <c r="D15" s="14" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>44</v>
@@ -1193,50 +1146,57 @@
         <v>48</v>
       </c>
       <c r="J15" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M15" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="N15" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="L15" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="M15" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="N15" s="15" t="s">
-        <v>69</v>
-      </c>
       <c r="O15" s="15" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="P15" s="15" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="Q15" s="15" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="R15" s="15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="S15" s="15" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="T15" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="U15" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="V15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W15" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>44</v>
@@ -1251,51 +1211,50 @@
         <v>48</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="M16" s="15" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="N16" s="15" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="O16" s="15" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="P16" s="15" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="Q16" s="15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="R16" s="15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="S16" s="15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="T16" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="U16" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>44</v>
@@ -1310,33 +1269,51 @@
         <v>48</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="P17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q17" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="R17" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="S17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="T17" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="U17" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>44</v>
@@ -1351,51 +1328,33 @@
         <v>48</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M18" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="N18" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="O18" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="P18" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q18" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="R18" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="S18" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="T18" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="U18" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>44</v>
@@ -1409,126 +1368,165 @@
       <c r="I19" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="15"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="J19" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q19" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="R19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="S19" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="T19" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="U19" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
-    </row>
-    <row r="21" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="L21" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M21" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="N21" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="O21" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="P21" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q21" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R21" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="S21" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="T21" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="U21" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N22" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="R22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="S22" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="T22" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U22" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
@@ -1545,10 +1543,10 @@
         <v>9</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -1565,10 +1563,10 @@
         <v>9</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -1585,10 +1583,10 @@
         <v>9</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -1605,10 +1603,10 @@
         <v>9</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -1621,6 +1619,15 @@
       <c r="N27" s="15"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
@@ -1632,15 +1639,6 @@
       <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>101</v>
-      </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
@@ -1656,10 +1654,10 @@
         <v>19</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -1676,10 +1674,10 @@
         <v>19</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
@@ -1696,10 +1694,10 @@
         <v>19</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
@@ -1716,10 +1714,10 @@
         <v>19</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
@@ -1736,10 +1734,10 @@
         <v>19</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
@@ -1756,10 +1754,10 @@
         <v>19</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
@@ -1772,6 +1770,15 @@
       <c r="N35" s="15"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>107</v>
+      </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
@@ -1782,94 +1789,85 @@
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
     </row>
-    <row r="37" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="K37" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="L37" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="M37" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="N37" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="O37" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="P37" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q37" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R37" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="S37" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="T37" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="U37" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+    </row>
+    <row r="38" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
+        <v>63</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L38" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M38" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N38" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="P38" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q38" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="R38" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="S38" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="T38" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U38" s="15" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
@@ -1886,10 +1884,10 @@
         <v>20</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
@@ -1902,7 +1900,15 @@
       <c r="N40" s="15"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D41" s="14"/>
+      <c r="A41" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
@@ -1914,15 +1920,7 @@
       <c r="N41" s="15"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>93</v>
-      </c>
+      <c r="D42" s="14"/>
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
@@ -1938,10 +1936,10 @@
         <v>21</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
@@ -1958,10 +1956,10 @@
         <v>21</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
@@ -1978,10 +1976,10 @@
         <v>21</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
@@ -1994,7 +1992,15 @@
       <c r="N45" s="15"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D46" s="14"/>
+      <c r="A46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>96</v>
+      </c>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
@@ -2006,15 +2012,7 @@
       <c r="N46" s="15"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>100</v>
-      </c>
+      <c r="D47" s="14"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
@@ -2026,7 +2024,15 @@
       <c r="N47" s="15"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D48" s="14"/>
+      <c r="A48" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
@@ -2038,15 +2044,7 @@
       <c r="N48" s="15"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>99</v>
-      </c>
+      <c r="D49" s="14"/>
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
@@ -2062,10 +2060,10 @@
         <v>17</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F50" s="15"/>
       <c r="G50" s="15"/>
@@ -2078,7 +2076,15 @@
       <c r="N50" s="15"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D51" s="14"/>
+      <c r="A51" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="F51" s="15"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
@@ -2090,15 +2096,7 @@
       <c r="N51" s="15"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>108</v>
-      </c>
+      <c r="D52" s="14"/>
       <c r="F52" s="15"/>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
@@ -2114,10 +2112,10 @@
         <v>18</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F53" s="15"/>
       <c r="G53" s="15"/>
@@ -2130,7 +2128,15 @@
       <c r="N53" s="15"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D54" s="14"/>
+      <c r="A54" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>109</v>
+      </c>
       <c r="F54" s="15"/>
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
@@ -2179,9 +2185,21 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D58" s="14"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D59" s="14"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D60" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>